<commit_message>
Minor changes to new files
</commit_message>
<xml_diff>
--- a/monitorizacionParalelo.xlsx
+++ b/monitorizacionParalelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignasi\Downloads\DocumentosUIB\2n - 2n - ACSI\Practica Tema 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0084A350-84DB-4080-9D2B-37AD797CEECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDFE504-F434-41D9-8BDF-5F9E4644C940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,19 @@
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4694,10 +4707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1441"/>
+  <dimension ref="A1:F1441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4706,9 +4719,10 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="69.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4722,7 +4736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -4735,8 +4749,12 @@
       <c r="D2" s="1">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>"Sobrecarga = 0,072 / 5 = " &amp; 0.072 / 5 *100</f>
+        <v>Sobrecarga = 0,072 / 5 = 1,44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -4750,7 +4768,7 @@
         <v>19.510000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -4764,7 +4782,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -4778,7 +4796,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -4792,7 +4810,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -4806,7 +4824,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -4820,7 +4838,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -4834,7 +4852,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -4848,7 +4866,7 @@
         <v>19.54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -4862,7 +4880,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -4876,7 +4894,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -4890,7 +4908,7 @@
         <v>19.54</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -4904,7 +4922,7 @@
         <v>19.52</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -4918,7 +4936,7 @@
         <v>19.53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>